<commit_message>
ng: Updates tas1 forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/2024/july_2024/kebbi/ng_lf_tas_2407_2_fts_kb.xlsx
+++ b/LF/TAS/Nigeria/2024/july_2024/kebbi/ng_lf_tas_2407_2_fts_kb.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\LF\TAS\Nigeria\2024\june_2024\Kebbi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Nigeria\2024\july_2024\kebbi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A731F7AC-DCCE-4C96-BF1A-322017DDAE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4A2D30-F1B8-49EB-99AC-A9FF61E9CF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -562,13 +562,13 @@
     <t>20</t>
   </si>
   <si>
-    <t>ng_lf_tas_2406_2_fts_kb_v31</t>
-  </si>
-  <si>
-    <t>ng_tas_fts_2406_kb_31</t>
-  </si>
-  <si>
-    <t>(June 2024) Kebbi - 2. TAS1 LF FTS Form V3</t>
+    <t>(July 2024) Kebbi - 2. TAS1 LF FTS Form V4</t>
+  </si>
+  <si>
+    <t>ng_lf_tas_2406_2_fts_kb_v4</t>
+  </si>
+  <si>
+    <t>ng_tas_fts_2406_kb_4</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1131,10 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1372,7 +1372,7 @@
         <v>100</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>107</v>
@@ -3664,7 +3664,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3691,10 +3691,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>97</v>

</xml_diff>